<commit_message>
Working on argument parser for command line interface
</commit_message>
<xml_diff>
--- a/Projects/testing/logs/Enrollment_Log.xlsx
+++ b/Projects/testing/logs/Enrollment_Log.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Enrollment_Log" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Enrollment_Log" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
   <si>
     <t>SubjectID</t>
   </si>
@@ -35,6 +35,27 @@
   </si>
   <si>
     <t>ResearchAssistantInitials</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>2017-11-05</t>
+  </si>
+  <si>
+    <t>18:47:54.570597</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>asd</t>
   </si>
 </sst>
 </file>
@@ -370,7 +391,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -401,6 +422,29 @@
         <v>6</v>
       </c>
     </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>